<commit_message>
Se agrega columna de nombre para codificar las fallas
Signed-off-by: jplaurent01 <josepablo.laurent@gmail.com>
</commit_message>
<xml_diff>
--- a/Proyecto/data_output/Simulaciones_Futuras_Fallas.xlsx
+++ b/Proyecto/data_output/Simulaciones_Futuras_Fallas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B261"/>
+  <dimension ref="A1:C261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>Fecha Predicha</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Causa Nombre</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -453,7 +458,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>29/10/2024</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -465,7 +475,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>17/10/2024</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -477,7 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -489,7 +509,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -501,7 +526,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>23/10/2024</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -513,7 +543,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>26/10/2024</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -525,7 +560,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>07/10/2024</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -537,7 +577,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>24/10/2024</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -549,7 +594,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -561,7 +611,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>18/10/2024</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -573,7 +628,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -585,7 +645,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -597,7 +662,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -609,7 +679,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -621,7 +696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -633,7 +713,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -645,7 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>10/10/2024</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -657,7 +747,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>21/10/2024</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -669,7 +764,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>27/10/2024</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -681,7 +781,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>14/10/2024</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -693,55 +798,80 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>28/10/2024</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>07/10/2024</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>25/10/2024</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>26/10/2024</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>03/10/2024</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -753,7 +883,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -765,7 +900,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>18/10/2024</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -777,7 +917,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -789,7 +934,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -801,7 +951,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>23/10/2024</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -813,7 +968,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>21/10/2024</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -825,7 +985,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -837,7 +1002,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>14/10/2024</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -849,7 +1019,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -861,7 +1036,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>15/10/2024</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -873,7 +1053,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>28/10/2024</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -885,7 +1070,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -897,7 +1087,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -909,7 +1104,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -921,7 +1121,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>13/10/2024</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -933,7 +1138,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -945,7 +1155,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>27/10/2024</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -957,7 +1172,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>24/10/2024</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -969,7 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>09/10/2024</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -981,7 +1206,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>10/10/2024</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -993,43 +1223,63 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>14/10/2024</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
           <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1291,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>18/10/2024</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1308,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>24/10/2024</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>29/09/2024</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1092,6 +1362,11 @@
           <t>13/10/2024</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1101,7 +1376,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1393,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1410,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>03/10/2024</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1427,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1444,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1461,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1478,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1495,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>07/10/2024</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1512,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1529,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>25/10/2024</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1546,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>21/10/2024</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1563,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>15/10/2024</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1580,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>30/09/2024</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1597,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>20/10/2024</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1614,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>26/10/2024</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1631,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>09/10/2024</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
@@ -1293,33 +1648,40 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>10/10/2024</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
-        </is>
-      </c>
+          <t>29/09/2024</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
-        </is>
-      </c>
+          <t>07/10/2024</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1329,9 +1691,10 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
-        </is>
-      </c>
+          <t>27/09/2024</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1341,9 +1704,10 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
-        </is>
-      </c>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1353,9 +1717,10 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
-        </is>
-      </c>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1365,9 +1730,10 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
-        </is>
-      </c>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1377,9 +1743,10 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
-        </is>
-      </c>
+          <t>09/10/2024</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1389,9 +1756,10 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
-        </is>
-      </c>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1401,9 +1769,10 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
-        </is>
-      </c>
+          <t>25/10/2024</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1413,9 +1782,10 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
-        </is>
-      </c>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1425,9 +1795,10 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
-        </is>
-      </c>
+          <t>21/10/2024</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1437,9 +1808,10 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
-        </is>
-      </c>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1449,9 +1821,10 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
-        </is>
-      </c>
+          <t>23/10/2024</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1461,9 +1834,10 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
-        </is>
-      </c>
+          <t>18/10/2024</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1473,9 +1847,10 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
-        </is>
-      </c>
+          <t>24/10/2024</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1485,9 +1860,10 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
-        </is>
-      </c>
+          <t>13/10/2024</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1497,9 +1873,10 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
-        </is>
-      </c>
+          <t>17/10/2024</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1509,9 +1886,10 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
-        </is>
-      </c>
+          <t>03/10/2024</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1521,9 +1899,10 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
-        </is>
-      </c>
+          <t>14/10/2024</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1536,6 +1915,7 @@
           <t>04/10/2024</t>
         </is>
       </c>
+      <c r="C92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1545,9 +1925,10 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
-        </is>
-      </c>
+          <t>28/09/2024</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1557,9 +1938,10 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
-        </is>
-      </c>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1569,9 +1951,10 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
-        </is>
-      </c>
+          <t>10/10/2024</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1581,55 +1964,76 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
-        </is>
-      </c>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>30/09/2024</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>29/09/2024</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1641,7 +2045,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1653,7 +2062,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>27/09/2024</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1665,7 +2079,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1677,7 +2096,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>17/10/2024</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1689,7 +2113,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>10/10/2024</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1701,7 +2130,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>18/10/2024</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1713,7 +2147,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>23/09/2024</t>
+          <t>09/10/2024</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1725,7 +2164,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1740,6 +2184,11 @@
           <t>25/09/2024</t>
         </is>
       </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -1749,7 +2198,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>13/10/2024</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1761,7 +2215,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1773,7 +2232,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1785,7 +2249,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>23/09/2024</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1797,7 +2266,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1809,7 +2283,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>26/09/2024</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1821,7 +2300,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>22/09/2024</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1833,7 +2317,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>24/09/2024</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1845,7 +2334,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>15/10/2024</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -1857,79 +2351,114 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>28/09/2024</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>27/10/2024</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>24/09/2024</t>
+          <t>03/10/2024</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>22/09/2024</t>
+          <t>28/10/2024</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>14/10/2024</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -1941,7 +2470,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>25/10/2024</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -1953,7 +2487,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>21/10/2024</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -1965,7 +2504,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>24/10/2024</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -1977,7 +2521,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>15/10/2024</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -1989,7 +2538,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>17/10/2024</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2555,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2572,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>18/10/2024</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2025,7 +2589,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2606,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>13/10/2024</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2623,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2061,7 +2640,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>10/10/2024</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2657,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>26/10/2024</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2085,7 +2674,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2691,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2708,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>09/10/2024</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2121,7 +2725,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2133,7 +2742,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2145,55 +2759,80 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>23/10/2024</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>29/10/2024</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>25/10/2024</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2208,6 +2847,11 @@
           <t>10/10/2024</t>
         </is>
       </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2217,7 +2861,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2878,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>27/10/2024</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2241,7 +2895,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2253,7 +2912,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>14/10/2024</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2265,7 +2929,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>17/10/2024</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2946,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2963,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>03/10/2024</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2980,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>24/10/2024</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2313,7 +2997,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2325,7 +3014,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>23/10/2024</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2337,7 +3031,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>09/10/2024</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2349,7 +3048,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>26/10/2024</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2361,7 +3065,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>07/10/2024</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2373,7 +3082,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>13/10/2024</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2385,7 +3099,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2397,7 +3116,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2409,7 +3133,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>21/10/2024</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2421,91 +3150,131 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>29/09/2024</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>28/09/2024</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>14/09/2024</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>26/09/2024</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>18/09/2024</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2517,7 +3286,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>23/09/2024</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2529,7 +3303,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>30/09/2024</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2541,7 +3320,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>25/09/2024</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2553,7 +3337,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>18/09/2024</t>
+          <t>15/09/2024</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2565,7 +3354,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2577,7 +3371,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>10/10/2024</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2589,7 +3388,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>16/09/2024</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2601,7 +3405,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>23/09/2024</t>
+          <t>19/09/2024</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2613,7 +3422,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
+          <t>17/09/2024</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2625,7 +3439,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>15/09/2024</t>
+          <t>09/10/2024</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2637,7 +3456,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>17/09/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2649,7 +3473,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>21/09/2024</t>
+          <t>22/09/2024</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2661,7 +3490,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2673,7 +3507,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>25/09/2024</t>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -2685,79 +3524,114 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>16/09/2024</t>
+          <t>27/09/2024</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>08/09/2024</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>23/08/2024</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>22/09/2024</t>
+          <t>28/08/2024</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>12/09/2024</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>05/09/2024</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>20/09/2024</t>
+          <t>04/09/2024</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2769,7 +3643,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>03/09/2024</t>
+          <t>15/09/2024</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2781,7 +3660,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>09/09/2024</t>
+          <t>14/09/2024</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2793,7 +3677,12 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>12/09/2024</t>
+          <t>29/08/2024</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2805,7 +3694,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>14/09/2024</t>
+          <t>03/09/2024</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2817,7 +3711,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>17/09/2024</t>
+          <t>25/08/2024</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2829,7 +3728,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>06/09/2024</t>
+          <t>11/09/2024</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2841,7 +3745,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>07/09/2024</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2853,7 +3762,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>24/08/2024</t>
+          <t>17/09/2024</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2865,7 +3779,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>11/09/2024</t>
+          <t>13/09/2024</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2877,7 +3796,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>28/08/2024</t>
+          <t>31/08/2024</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2889,7 +3813,12 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>26/08/2024</t>
+          <t>02/09/2024</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2901,7 +3830,12 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>07/09/2024</t>
+          <t>21/08/2024</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2913,7 +3847,12 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>27/08/2024</t>
+          <t>10/09/2024</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2925,7 +3864,12 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>20/08/2024</t>
+          <t>30/08/2024</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2940,6 +3884,11 @@
           <t>22/08/2024</t>
         </is>
       </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -2952,6 +3901,11 @@
           <t>01/09/2024</t>
         </is>
       </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -2961,7 +3915,12 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>04/09/2024</t>
+          <t>26/08/2024</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2973,7 +3932,12 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>25/08/2024</t>
+          <t>16/09/2024</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -2985,43 +3949,63 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>13/09/2024</t>
+          <t>27/08/2024</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>05/09/2024</t>
+          <t>29/09/2024</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>21/08/2024</t>
+          <t>18/10/2024</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3033,7 +4017,12 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>09/10/2024</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3045,7 +4034,12 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>27/09/2024</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3057,7 +4051,12 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>28/09/2024</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3069,7 +4068,12 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3081,7 +4085,12 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3093,7 +4102,12 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>26/09/2024</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3105,7 +4119,12 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3117,7 +4136,12 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3129,7 +4153,12 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>21/10/2024</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3141,7 +4170,12 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3153,7 +4187,12 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>10/10/2024</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3165,7 +4204,12 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3177,7 +4221,12 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
+          <t>24/10/2024</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3189,7 +4238,12 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3201,7 +4255,12 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>20/10/2024</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3213,7 +4272,12 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>07/10/2024</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3225,7 +4289,12 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3237,7 +4306,12 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>15/10/2024</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3249,7 +4323,12 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>14/10/2024</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3261,7 +4340,12 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>23/10/2024</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3273,31 +4357,46 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>409</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>17/10/2024</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>409</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>07/10/2024</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3309,7 +4408,12 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>14/10/2024</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3321,7 +4425,12 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3333,7 +4442,12 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3345,7 +4459,12 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>29/10/2024</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3357,7 +4476,12 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3369,7 +4493,12 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>13/10/2024</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3381,7 +4510,12 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>21/10/2024</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3393,7 +4527,12 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>23/10/2024</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3405,7 +4544,12 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>26/10/2024</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3417,7 +4561,12 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3429,7 +4578,12 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3441,7 +4595,12 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>18/10/2024</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3453,7 +4612,12 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>27/10/2024</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3465,7 +4629,12 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3477,7 +4646,12 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3489,7 +4663,12 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3501,7 +4680,12 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>03/10/2024</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3513,7 +4697,12 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3525,7 +4714,12 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>06/10/2024</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3537,7 +4731,12 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>15/10/2024</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3549,7 +4748,12 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>28/10/2024</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -3562,6 +4766,11 @@
       <c r="B261" t="inlineStr">
         <is>
           <t>25/10/2024</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se actualiza version del codigo
Signed-off-by: jplaurent01 <josepablo.laurent@gmail.com>
</commit_message>
<xml_diff>
--- a/Proyecto/data_output/Simulaciones_Futuras_Fallas.xlsx
+++ b/Proyecto/data_output/Simulaciones_Futuras_Fallas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C261"/>
+  <dimension ref="A1:C258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>29/10/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -730,7 +730,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -810,51 +810,51 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>101</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Momentaneas</t>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>101</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Momentaneas</t>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>101</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Momentaneas</t>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>28/10/2024</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>27/10/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>29/09/2024</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>28/09/2024</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1626,36 +1626,28 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Primarios reventados o dañados</t>
-        </is>
-      </c>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Primarios reventados o dañados</t>
-        </is>
-      </c>
+          <t>24/10/2024</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1665,7 +1657,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -1678,7 +1670,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
@@ -1691,7 +1683,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
@@ -1704,7 +1696,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
@@ -1717,7 +1709,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
@@ -1730,7 +1722,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
@@ -1743,7 +1735,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
@@ -1756,7 +1748,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -1769,7 +1761,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -1782,7 +1774,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>28/09/2024</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -1795,7 +1787,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -1808,7 +1800,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>27/09/2024</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -1821,7 +1813,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -1834,7 +1826,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -1847,7 +1839,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -1860,7 +1852,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
@@ -1873,7 +1865,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
@@ -1886,7 +1878,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -1899,7 +1891,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -1907,67 +1899,87 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr"/>
+          <t>26/09/2024</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr"/>
+          <t>13/10/2024</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr"/>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr"/>
+          <t>23/09/2024</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr"/>
+          <t>05/10/2024</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Baja frecuencia</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1977,7 +1989,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>29/09/2024</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -1994,7 +2006,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2028,7 +2040,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2045,7 +2057,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2062,7 +2074,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2079,7 +2091,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2096,7 +2108,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2113,7 +2125,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>24/09/2024</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2130,7 +2142,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2147,7 +2159,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>27/09/2024</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2164,7 +2176,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2181,7 +2193,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>25/09/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2198,7 +2210,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2215,7 +2227,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2232,7 +2244,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2249,7 +2261,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>23/09/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2266,7 +2278,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>25/09/2024</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2283,7 +2295,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2295,68 +2307,68 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>22/09/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Baja frecuencia</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>24/09/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Baja frecuencia</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Baja frecuencia</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Baja frecuencia</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2368,7 +2380,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -2385,7 +2397,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -2402,7 +2414,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2419,7 +2431,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -2436,7 +2448,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2453,7 +2465,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2470,7 +2482,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2487,7 +2499,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2504,7 +2516,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2521,7 +2533,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2538,7 +2550,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>28/10/2024</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2555,7 +2567,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2572,7 +2584,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -2589,7 +2601,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2606,7 +2618,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -2623,7 +2635,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2640,7 +2652,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>27/10/2024</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -2657,7 +2669,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2674,7 +2686,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -2691,7 +2703,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -2703,68 +2715,68 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>27/10/2024</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -2776,7 +2788,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -2793,7 +2805,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -2810,7 +2822,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -2827,7 +2839,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -2844,7 +2856,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2861,7 +2873,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -2878,7 +2890,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -2895,7 +2907,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -2912,7 +2924,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>29/10/2024</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -2929,7 +2941,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -2946,7 +2958,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -2963,7 +2975,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -2980,7 +2992,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -2997,7 +3009,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3014,7 +3026,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3031,7 +3043,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3048,7 +3060,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>28/10/2024</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3065,7 +3077,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3077,85 +3089,85 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>23/09/2024</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>29/09/2024</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3179,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>27/09/2024</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -3184,7 +3196,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>22/09/2024</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -3201,7 +3213,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>14/09/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -3218,7 +3230,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
+          <t>25/09/2024</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -3235,7 +3247,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -3252,7 +3264,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>18/09/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3269,7 +3281,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3286,7 +3298,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>23/09/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3303,7 +3315,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3320,7 +3332,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>25/09/2024</t>
+          <t>19/09/2024</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3337,7 +3349,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>15/09/2024</t>
+          <t>20/09/2024</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -3354,7 +3366,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>24/09/2024</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3371,7 +3383,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3388,7 +3400,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>16/09/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -3405,7 +3417,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>15/09/2024</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -3422,7 +3434,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>17/09/2024</t>
+          <t>26/09/2024</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3439,7 +3451,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>21/09/2024</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3456,7 +3468,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>18/09/2024</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3473,7 +3485,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>22/09/2024</t>
+          <t>28/09/2024</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -3490,7 +3502,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>16/09/2024</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3507,7 +3519,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -3519,17 +3531,17 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>03/09/2024</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -3541,7 +3553,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>08/09/2024</t>
+          <t>16/09/2024</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -3558,7 +3570,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>23/08/2024</t>
+          <t>12/09/2024</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -3575,7 +3587,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>28/08/2024</t>
+          <t>10/09/2024</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -3592,7 +3604,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>12/09/2024</t>
+          <t>07/09/2024</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -3609,7 +3621,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>05/09/2024</t>
+          <t>28/08/2024</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -3626,7 +3638,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>04/09/2024</t>
+          <t>11/09/2024</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -3643,7 +3655,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>15/09/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -3660,7 +3672,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>14/09/2024</t>
+          <t>05/09/2024</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -3677,7 +3689,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>20/08/2024</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -3694,7 +3706,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>03/09/2024</t>
+          <t>24/08/2024</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -3711,7 +3723,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>25/08/2024</t>
+          <t>22/08/2024</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -3728,7 +3740,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>11/09/2024</t>
+          <t>21/08/2024</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -3745,7 +3757,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>07/09/2024</t>
+          <t>23/08/2024</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -3762,7 +3774,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>17/09/2024</t>
+          <t>15/09/2024</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -3796,7 +3808,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>31/08/2024</t>
+          <t>01/09/2024</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -3813,7 +3825,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>29/08/2024</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -3830,7 +3842,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>21/08/2024</t>
+          <t>26/08/2024</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -3847,7 +3859,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>10/09/2024</t>
+          <t>17/09/2024</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -3864,7 +3876,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>30/08/2024</t>
+          <t>09/09/2024</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -3881,7 +3893,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>22/08/2024</t>
+          <t>25/08/2024</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -3893,68 +3905,68 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>01/09/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>26/08/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>16/09/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>27/08/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -3966,7 +3978,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>26/09/2024</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -3983,7 +3995,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -4000,7 +4012,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>28/09/2024</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -4017,7 +4029,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -4034,7 +4046,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -4051,7 +4063,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -4068,7 +4080,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -4085,7 +4097,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -4102,7 +4114,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
+          <t>29/09/2024</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4119,7 +4131,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -4136,7 +4148,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>27/09/2024</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -4153,7 +4165,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -4170,7 +4182,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -4187,7 +4199,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -4204,7 +4216,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -4221,7 +4233,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -4238,7 +4250,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4255,7 +4267,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -4272,7 +4284,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -4289,7 +4301,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -4301,68 +4313,68 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>409</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>409</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>409</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>409</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérdida de alimentador por causa desconocida</t>
         </is>
       </c>
     </row>
@@ -4374,7 +4386,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -4391,7 +4403,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>27/10/2024</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -4408,7 +4420,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -4425,7 +4437,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -4442,7 +4454,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -4459,7 +4471,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -4476,7 +4488,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -4493,7 +4505,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -4510,7 +4522,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -4527,7 +4539,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -4544,7 +4556,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -4561,7 +4573,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -4578,7 +4590,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -4595,7 +4607,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -4612,7 +4624,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -4629,7 +4641,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -4646,7 +4658,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -4663,7 +4675,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -4680,7 +4692,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -4714,61 +4726,10 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
-        <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
-        </is>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="inlineStr">
-        <is>
-          <t>409</t>
-        </is>
-      </c>
-      <c r="B259" t="inlineStr">
-        <is>
-          <t>15/10/2024</t>
-        </is>
-      </c>
-      <c r="C259" t="inlineStr">
-        <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
-        </is>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="inlineStr">
-        <is>
-          <t>409</t>
-        </is>
-      </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t>28/10/2024</t>
-        </is>
-      </c>
-      <c r="C260" t="inlineStr">
-        <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
-        </is>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="inlineStr">
-        <is>
-          <t>409</t>
-        </is>
-      </c>
-      <c r="B261" t="inlineStr">
-        <is>
-          <t>25/10/2024</t>
-        </is>
-      </c>
-      <c r="C261" t="inlineStr">
         <is>
           <t>Pérdida de alimentador por causa desconocida</t>
         </is>

</xml_diff>

<commit_message>
Se agrega prueba de modelos
Signed-off-by: jplaurent01 <josepablo.laurent@gmail.com>
</commit_message>
<xml_diff>
--- a/Proyecto/data_output/Simulaciones_Futuras_Fallas.xlsx
+++ b/Proyecto/data_output/Simulaciones_Futuras_Fallas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C258"/>
+  <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>27/10/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,7 +475,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -509,7 +509,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>29/10/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -730,7 +730,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>28/10/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -832,7 +832,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -861,17 +861,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>101</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Momentaneas</t>
+          <t>No identificada</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1104,7 +1104,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>27/10/2024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>28/10/2024</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1235,85 +1235,85 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Primarios reventados o dañados</t>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Primarios reventados o dañados</t>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Primarios reventados o dañados</t>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Primarios reventados o dañados</t>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>106</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Primarios reventados o dañados</t>
+          <t>Momentaneas</t>
         </is>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>28/09/2024</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>29/09/2024</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1626,80 +1626,104 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr"/>
+          <t>23/10/2024</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr"/>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr"/>
+          <t>30/09/2024</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr"/>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr"/>
+          <t>12/10/2024</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>108</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr"/>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Primarios reventados o dañados</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1709,7 +1733,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
@@ -1722,7 +1746,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
@@ -1735,7 +1759,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
@@ -1748,7 +1772,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -1761,7 +1785,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -1774,7 +1798,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -1787,7 +1811,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>27/09/2024</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -1800,7 +1824,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -1813,7 +1837,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -1826,7 +1850,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -1839,7 +1863,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -1852,7 +1876,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
@@ -1865,7 +1889,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
@@ -1878,7 +1902,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -1891,7 +1915,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -1899,138 +1923,106 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Baja frecuencia</t>
-        </is>
-      </c>
+          <t>25/10/2024</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Baja frecuencia</t>
-        </is>
-      </c>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Baja frecuencia</t>
-        </is>
-      </c>
+          <t>02/10/2024</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>23/09/2024</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Baja frecuencia</t>
-        </is>
-      </c>
+          <t>11/10/2024</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Baja frecuencia</t>
-        </is>
-      </c>
+          <t>19/10/2024</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Baja frecuencia</t>
-        </is>
-      </c>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Baja frecuencia</t>
-        </is>
-      </c>
+          <t>16/10/2024</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>204</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Baja frecuencia</t>
-        </is>
-      </c>
+          <t>04/10/2024</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2040,7 +2032,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2057,7 +2049,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2074,7 +2066,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>27/09/2024</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2108,7 +2100,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2125,7 +2117,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>24/09/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2142,7 +2134,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2159,7 +2151,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2176,7 +2168,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2193,7 +2185,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>29/09/2024</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2210,7 +2202,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>26/09/2024</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2227,7 +2219,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2244,7 +2236,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>22/09/2024</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2261,7 +2253,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>23/09/2024</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2278,7 +2270,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>25/09/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2295,7 +2287,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>25/09/2024</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2307,136 +2299,136 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>28/09/2024</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>24/09/2024</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Maniobras por operación programada</t>
+          <t>Baja frecuencia</t>
         </is>
       </c>
     </row>
@@ -2448,7 +2440,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2465,7 +2457,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2482,7 +2474,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2499,7 +2491,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -2516,7 +2508,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2533,7 +2525,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2550,7 +2542,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2567,7 +2559,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>28/10/2024</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2584,7 +2576,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -2601,7 +2593,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2618,7 +2610,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -2635,7 +2627,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2652,7 +2644,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -2669,7 +2661,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2686,7 +2678,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -2703,7 +2695,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -2715,136 +2707,136 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>306</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Maniobras por operación  NO programada -INT-</t>
+          <t>Maniobras por operación programada</t>
         </is>
       </c>
     </row>
@@ -2856,7 +2848,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -2873,7 +2865,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>28/10/2024</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -2890,7 +2882,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -2907,7 +2899,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -2924,7 +2916,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>29/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -2941,7 +2933,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -2958,7 +2950,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -2975,7 +2967,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -2992,7 +2984,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>29/10/2024</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3009,7 +3001,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3026,7 +3018,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3043,7 +3035,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3060,7 +3052,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>28/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3077,7 +3069,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3089,7 +3081,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -3099,177 +3091,177 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>23/09/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>14/10/2024</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>22/09/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>25/09/2024</t>
+          <t>25/10/2024</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>27/10/2024</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>307</t>
+          <t>306</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Maniobras por operación NO programada -EXT-</t>
+          <t>Maniobras por operación  NO programada -INT-</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3273,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>15/09/2024</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -3298,7 +3290,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>18/09/2024</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -3315,7 +3307,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>29/09/2024</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3332,7 +3324,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>21/09/2024</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -3349,7 +3341,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>20/09/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -3366,7 +3358,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>24/09/2024</t>
+          <t>25/09/2024</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -3383,7 +3375,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>17/09/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -3400,7 +3392,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -3417,7 +3409,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>15/09/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -3434,7 +3426,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
+          <t>14/09/2024</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -3451,7 +3443,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>21/09/2024</t>
+          <t>19/09/2024</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -3468,7 +3460,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>18/09/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -3485,7 +3477,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>26/09/2024</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -3502,7 +3494,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>16/09/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -3519,7 +3511,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>24/09/2024</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -3531,119 +3523,119 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>03/09/2024</t>
+          <t>08/10/2024</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>16/09/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>12/09/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>10/09/2024</t>
+          <t>28/09/2024</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>07/09/2024</t>
+          <t>22/09/2024</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>28/08/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>402</t>
+          <t>307</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>11/09/2024</t>
+          <t>23/09/2024</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes internos</t>
+          <t>Maniobras por operación NO programada -EXT-</t>
         </is>
       </c>
     </row>
@@ -3655,7 +3647,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>13/09/2024</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -3672,7 +3664,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>05/09/2024</t>
+          <t>12/09/2024</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -3689,7 +3681,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>20/08/2024</t>
+          <t>16/09/2024</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -3706,7 +3698,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>24/08/2024</t>
+          <t>20/08/2024</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -3723,7 +3715,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>22/08/2024</t>
+          <t>04/09/2024</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -3740,7 +3732,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>21/08/2024</t>
+          <t>22/08/2024</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -3757,7 +3749,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>23/08/2024</t>
+          <t>30/08/2024</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -3774,7 +3766,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>15/09/2024</t>
+          <t>06/09/2024</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -3791,7 +3783,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>13/09/2024</t>
+          <t>01/09/2024</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -3808,7 +3800,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>01/09/2024</t>
+          <t>23/08/2024</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -3825,7 +3817,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>29/08/2024</t>
+          <t>28/08/2024</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -3842,7 +3834,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>26/08/2024</t>
+          <t>25/08/2024</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -3859,7 +3851,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>17/09/2024</t>
+          <t>21/08/2024</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -3876,7 +3868,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>09/09/2024</t>
+          <t>10/09/2024</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -3893,7 +3885,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>25/08/2024</t>
+          <t>14/09/2024</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -3905,153 +3897,153 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>27/08/2024</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>24/08/2024</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>05/09/2024</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>11/10/2024</t>
+          <t>11/09/2024</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>26/09/2024</t>
+          <t>31/08/2024</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>04/10/2024</t>
+          <t>09/09/2024</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>28/09/2024</t>
+          <t>03/09/2024</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>26/08/2024</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>402</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>30/09/2024</t>
+          <t>08/09/2024</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Pérd. de alimentador por agentes externos</t>
+          <t>Pérd. de alimentador por agentes internos</t>
         </is>
       </c>
     </row>
@@ -4080,7 +4072,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>05/10/2024</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -4097,7 +4089,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>27/09/2024</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -4114,7 +4106,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>29/09/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -4131,7 +4123,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -4148,7 +4140,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>27/09/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -4165,7 +4157,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>07/10/2024</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -4182,7 +4174,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>17/10/2024</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -4199,7 +4191,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -4216,7 +4208,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>29/09/2024</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -4233,7 +4225,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -4250,7 +4242,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>22/10/2024</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -4267,7 +4259,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>30/09/2024</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -4284,7 +4276,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>28/09/2024</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -4301,7 +4293,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>06/10/2024</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -4313,102 +4305,102 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>18/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>19/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>12/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>26/09/2024</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>403</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>27/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Pérdida de alimentador por causa desconocida</t>
+          <t>Pérd. de alimentador por agentes externos</t>
         </is>
       </c>
     </row>
@@ -4420,7 +4412,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>07/10/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -4437,7 +4429,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>15/10/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -4454,7 +4446,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>10/10/2024</t>
+          <t>19/10/2024</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -4471,7 +4463,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>08/10/2024</t>
+          <t>11/10/2024</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -4488,7 +4480,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>15/10/2024</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -4505,7 +4497,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>20/10/2024</t>
+          <t>09/10/2024</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -4522,7 +4514,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>13/10/2024</t>
+          <t>10/10/2024</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -4539,7 +4531,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>06/10/2024</t>
+          <t>26/10/2024</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -4556,7 +4548,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>09/10/2024</t>
+          <t>04/10/2024</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -4573,7 +4565,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>16/10/2024</t>
+          <t>20/10/2024</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -4590,7 +4582,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>14/10/2024</t>
+          <t>18/10/2024</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -4607,7 +4599,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>03/10/2024</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -4624,7 +4616,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>05/10/2024</t>
+          <t>13/10/2024</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -4641,7 +4633,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>17/10/2024</t>
+          <t>23/10/2024</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -4658,7 +4650,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>24/10/2024</t>
+          <t>16/10/2024</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -4675,7 +4667,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>26/10/2024</t>
+          <t>28/10/2024</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -4692,7 +4684,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>25/10/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -4709,7 +4701,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>22/10/2024</t>
+          <t>24/10/2024</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -4726,10 +4718,78 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>23/10/2024</t>
+          <t>12/10/2024</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>409</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>08/10/2024</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>409</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>25/10/2024</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>409</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>22/10/2024</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Pérdida de alimentador por causa desconocida</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>409</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>27/10/2024</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
         <is>
           <t>Pérdida de alimentador por causa desconocida</t>
         </is>

</xml_diff>